<commit_message>
HR Coordinator predefined criteria
</commit_message>
<xml_diff>
--- a/vacancie_01/_static/applicants/metadata2.xlsx
+++ b/vacancie_01/_static/applicants/metadata2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/21540b8bb60256b0/Bachelorarbeit/docs/job_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{55050E14-E149-4C1E-88D5-FFCE983D53C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC8CA05-F8D6-4435-8634-A4E2B8DAF8C6}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{55050E14-E149-4C1E-88D5-FFCE983D53C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3996D27F-9D6E-47E3-B4F2-4A5DE5DD88E0}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4105B825-04A9-43F3-958D-3B952C1641F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4105B825-04A9-43F3-958D-3B952C1641F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1508,7 +1508,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,7 +1725,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>3</v>
@@ -2569,8 +2569,8 @@
       <c r="B17" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>40</v>
+      <c r="C17" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>58</v>
@@ -2765,7 +2765,7 @@
         <v>79</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>58</v>
@@ -3350,7 +3350,7 @@
         <v>98</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>163</v>
@@ -3480,7 +3480,7 @@
         <v>103</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>104</v>

</xml_diff>